<commit_message>
Risikomangement V3 Skala verbessert
</commit_message>
<xml_diff>
--- a/Risikomanagement/20160405_Risikomanagement_KC_V3.xlsx
+++ b/Risikomanagement/20160405_Risikomanagement_KC_V3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="3880" yWindow="1660" windowWidth="24800" windowHeight="15880"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="131">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -437,6 +437,15 @@
   </si>
   <si>
     <t>1,2,14,24,32,33</t>
+  </si>
+  <si>
+    <t>[ 1 - 5 ]</t>
+  </si>
+  <si>
+    <t>Cx * Dx</t>
+  </si>
+  <si>
+    <t>präventiv / reaktiv</t>
   </si>
 </sst>
 </file>
@@ -756,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -919,14 +928,32 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -980,8 +1007,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="3"/>
-      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1501,7 +1528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1509,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1527,93 +1554,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="H3" s="1"/>
+    <row r="3" spans="1:8" s="58" customFormat="1" ht="15.75" customHeight="1">
+      <c r="D3" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="62" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A5" s="8">
+    <row r="6" spans="1:8" ht="38.25" customHeight="1">
+      <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="8">
-        <v>3</v>
-      </c>
-      <c r="E5" s="8">
-        <v>3</v>
-      </c>
-      <c r="F5" s="11">
-        <f t="shared" ref="F5:F29" si="0">D5*E5</f>
-        <v>9</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="51" customHeight="1">
-      <c r="A6" s="8">
-        <v>2</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="D6" s="8">
         <v>3</v>
@@ -1622,320 +1636,320 @@
         <v>3</v>
       </c>
       <c r="F6" s="11">
+        <f t="shared" ref="F6:F30" si="0">D6*E6</f>
+        <v>9</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" customHeight="1">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3</v>
+      </c>
+      <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="63.75" customHeight="1">
-      <c r="A7" s="8">
+    <row r="8" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D8" s="8">
         <v>4</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="51" customHeight="1">
-      <c r="A8" s="8">
+    <row r="9" spans="1:8" ht="51" customHeight="1">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B9" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D9" s="8">
         <v>3</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E9" s="8">
         <v>4</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F9" s="11">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="63.75" customHeight="1">
-      <c r="A9" s="8">
+    <row r="10" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A10" s="8">
         <v>5</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B10" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D10" s="8">
         <v>2</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E10" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F10" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A10" s="8">
+    <row r="11" spans="1:8" ht="38.25" customHeight="1">
+      <c r="A11" s="8">
         <v>6</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B11" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D11" s="8">
         <v>5</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E11" s="8">
         <v>4</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F11" s="11">
         <v>20</v>
       </c>
-      <c r="G10" s="49" t="s">
+      <c r="G11" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H11" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="63.75" customHeight="1">
-      <c r="A11" s="8">
+    <row r="12" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A12" s="8">
         <v>7</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C12" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D12" s="8">
         <v>2</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E12" s="8">
         <v>2</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F12" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H12" s="35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="63.75" customHeight="1">
-      <c r="A12" s="8">
+    <row r="13" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A13" s="8">
         <v>8</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B13" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C13" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="8">
         <v>1</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E13" s="8">
         <v>3</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F13" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H13" s="35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="51" customHeight="1">
-      <c r="A13" s="8">
+    <row r="14" spans="1:8" ht="51" customHeight="1">
+      <c r="A14" s="8">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B14" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C14" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <v>1</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E14" s="8">
         <v>1</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F14" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H14" s="35" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="51" customHeight="1">
-      <c r="A14" s="8">
+    <row r="15" spans="1:8" ht="51" customHeight="1">
+      <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D15" s="8">
         <v>3</v>
-      </c>
-      <c r="E14" s="8">
-        <v>4</v>
-      </c>
-      <c r="F14" s="11">
-        <v>12</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A15" s="8">
-        <v>11</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="8">
-        <v>2</v>
       </c>
       <c r="E15" s="8">
         <v>4</v>
       </c>
       <c r="F15" s="11">
+        <v>12</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="38.25" customHeight="1">
+      <c r="A16" s="8">
+        <v>11</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2</v>
+      </c>
+      <c r="E16" s="8">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H16" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="51" customHeight="1">
-      <c r="A16" s="8">
+    <row r="17" spans="1:8" ht="51" customHeight="1">
+      <c r="A17" s="8">
         <v>12</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D17" s="8">
         <v>2</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E17" s="8">
         <v>3</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F17" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G16" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A17" s="8">
-        <v>13</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="8">
-        <v>2</v>
-      </c>
-      <c r="E17" s="8">
-        <v>2</v>
-      </c>
-      <c r="F17" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
       <c r="G17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="51" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="38.25" customHeight="1">
       <c r="A18" s="8">
-        <v>14</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D18" s="8">
         <v>2</v>
@@ -1951,207 +1965,207 @@
         <v>20</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="51" customHeight="1">
       <c r="A19" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D19" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="38.25" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="51" customHeight="1">
       <c r="A20" s="8">
-        <v>16</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>42</v>
+        <v>15</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="D20" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="8">
         <v>3</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="51" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="38.25" customHeight="1">
       <c r="A21" s="8">
-        <v>17</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>45</v>
+        <v>16</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="D21" s="8">
         <v>2</v>
       </c>
       <c r="E21" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="63.75" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="51" customHeight="1">
       <c r="A22" s="8">
-        <v>18</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>47</v>
+        <v>17</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="8">
         <v>4</v>
       </c>
       <c r="F22" s="11">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="63.75" customHeight="1">
       <c r="A23" s="8">
-        <v>19</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D23" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F23" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="76.5" customHeight="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="63.75" customHeight="1">
       <c r="A24" s="8">
-        <v>20</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="51" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="76.5" customHeight="1">
       <c r="A25" s="8">
-        <v>21</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>95</v>
+        <v>20</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D25" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E25" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="35" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="51" customHeight="1">
       <c r="A26" s="8">
-        <v>22</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>58</v>
+        <v>21</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>95</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>
@@ -2166,285 +2180,286 @@
       <c r="G26" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="63.75" customHeight="1">
+      <c r="H26" s="35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="51" customHeight="1">
       <c r="A27" s="8">
-        <v>23</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D27" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F27" s="11">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="76.5" customHeight="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="63.75" customHeight="1">
       <c r="A28" s="8">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D28" s="8">
         <v>3</v>
       </c>
       <c r="E28" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" s="11">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="38.25" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="76.5" customHeight="1">
       <c r="A29" s="8">
-        <v>25</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>97</v>
+        <v>24</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="D29" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H29" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="38.25" customHeight="1">
+      <c r="A30" s="8">
+        <v>25</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8">
+        <v>5</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="51" customHeight="1">
-      <c r="A30" s="8">
+    <row r="31" spans="1:8" ht="51" customHeight="1">
+      <c r="A31" s="8">
         <v>26</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D31" s="8">
         <v>3</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E31" s="8">
         <v>1</v>
       </c>
-      <c r="F30" s="11">
-        <f>D30*E30</f>
+      <c r="F31" s="11">
+        <f>D31*E31</f>
         <v>3</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G31" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H31" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="79.5" customHeight="1">
-      <c r="A31" s="2">
+    <row r="32" spans="1:8" ht="79.5" customHeight="1">
+      <c r="A32" s="2">
         <v>27</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B32" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <v>3</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E32" s="2">
         <v>5</v>
       </c>
-      <c r="F31" s="38">
+      <c r="F32" s="38">
         <v>15</v>
       </c>
-      <c r="G31" s="45" t="s">
+      <c r="G32" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="H31" s="39" t="s">
+      <c r="H32" s="39" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="67.5" customHeight="1">
-      <c r="A32" s="2">
+    <row r="33" spans="1:8" ht="67.5" customHeight="1">
+      <c r="A33" s="2">
         <v>28</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B33" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D32" s="2">
-        <v>4</v>
-      </c>
-      <c r="E32" s="2">
-        <v>2</v>
-      </c>
-      <c r="F32" s="38">
-        <f>D32*E32</f>
-        <v>8</v>
-      </c>
-      <c r="G32" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="58.5" customHeight="1">
-      <c r="A33" s="2">
-        <v>29</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D33" s="2">
         <v>4</v>
       </c>
       <c r="E33" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33" s="38">
         <f>D33*E33</f>
+        <v>8</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="58.5" customHeight="1">
+      <c r="A34" s="2">
+        <v>29</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4</v>
+      </c>
+      <c r="F34" s="38">
+        <f>D34*E34</f>
         <v>16</v>
       </c>
-      <c r="G33" s="42" t="s">
+      <c r="G34" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H34" s="41" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="64.5" customHeight="1">
-      <c r="A34" s="2">
+    <row r="35" spans="1:8" ht="64.5" customHeight="1">
+      <c r="A35" s="2">
         <v>30</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B35" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="52" t="s">
+      <c r="C35" s="52" t="s">
         <v>110</v>
-      </c>
-      <c r="D34" s="2">
-        <v>3</v>
-      </c>
-      <c r="E34" s="2">
-        <v>3</v>
-      </c>
-      <c r="F34" s="38">
-        <v>9</v>
-      </c>
-      <c r="G34" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="53" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="70.5" customHeight="1">
-      <c r="A35" s="2">
-        <v>31</v>
-      </c>
-      <c r="B35" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>118</v>
       </c>
       <c r="D35" s="2">
         <v>3</v>
       </c>
       <c r="E35" s="2">
+        <v>3</v>
+      </c>
+      <c r="F35" s="38">
+        <v>9</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="70.5" customHeight="1">
+      <c r="A36" s="2">
+        <v>31</v>
+      </c>
+      <c r="B36" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2">
         <v>4</v>
       </c>
-      <c r="F35" s="38">
+      <c r="F36" s="38">
         <v>12</v>
       </c>
-      <c r="G35" s="45" t="s">
+      <c r="G36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H35" s="54" t="s">
+      <c r="H36" s="54" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A36" s="2">
-        <v>32</v>
-      </c>
-      <c r="B36" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="2">
-        <v>2</v>
-      </c>
-      <c r="E36" s="2">
-        <v>3</v>
-      </c>
-      <c r="F36" s="38">
-        <v>6</v>
-      </c>
-      <c r="G36" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="54" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="66.75" customHeight="1">
       <c r="A37" s="2">
-        <v>33</v>
-      </c>
-      <c r="B37" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>124</v>
+        <v>32</v>
+      </c>
+      <c r="B37" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="52" t="s">
+        <v>123</v>
       </c>
       <c r="D37" s="2">
         <v>2</v>
@@ -2455,22 +2470,38 @@
       <c r="F37" s="38">
         <v>6</v>
       </c>
-      <c r="G37" s="55" t="s">
+      <c r="G37" s="40" t="s">
         <v>17</v>
       </c>
       <c r="H37" s="54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A38" s="2">
+        <v>33</v>
+      </c>
+      <c r="B38" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3</v>
+      </c>
+      <c r="F38" s="38">
+        <v>6</v>
+      </c>
+      <c r="G38" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="54" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1">
       <c r="A39" s="2"/>
@@ -2493,19 +2524,34 @@
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A41" s="19"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
       <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A42" s="19"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="H42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6 F1:G990">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="B7 F1:G2 F4:G991 G3">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2555,7 +2601,7 @@
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="105" customHeight="1">
-      <c r="A2" s="60"/>
+      <c r="A2" s="61"/>
       <c r="B2" s="20" t="s">
         <v>71</v>
       </c>
@@ -2578,7 +2624,7 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" ht="105" customHeight="1">
-      <c r="A3" s="59"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="20" t="s">
         <v>72</v>
       </c>
@@ -2607,7 +2653,7 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" ht="105" customHeight="1">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="20" t="s">
         <v>73</v>
       </c>
@@ -2638,7 +2684,7 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="105" customHeight="1">
-      <c r="A5" s="59"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="29" t="s">
         <v>74</v>
       </c>
@@ -2667,7 +2713,7 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="105" customHeight="1">
-      <c r="A6" s="59"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="20" t="s">
         <v>75</v>
       </c>
@@ -2725,11 +2771,11 @@
     <row r="8" spans="1:17" ht="105" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4742,7 +4788,7 @@
     <mergeCell ref="C8:G8"/>
   </mergeCells>
   <conditionalFormatting sqref="B102">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(B102))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>